<commit_message>
Fix template placeholder mismatches for quotation & invoice
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E543"/>
+  <dimension ref="A1:E636"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15094,6 +15094,2517 @@
         </is>
       </c>
     </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:13:48</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E544" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:13:48</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E545" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:13:57</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E546" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:13:58</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E547" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:02</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:19</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:22</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E550" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:25</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E551" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:26</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E552" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:39</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E553" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:42</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E554" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:46</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E555" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:54</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:14:57</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E557" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:20:41</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E558" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:20:56</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E559" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:05</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E560" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:11</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E561" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:13</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E562" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:13</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E563" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:15</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E564" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:16</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E565" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:16</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E566" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:17</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E567" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:21:28</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E568" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:25:29</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E569" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:25:31</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E570" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:25:33</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E571" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:30:21</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E572" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:30:22</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E573" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:30:24</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E574" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:30:29</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E575" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:30:30</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:32:35</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E577" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:32:35</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E578" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:32:36</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E579" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:32:39</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E580" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:33:28</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E581" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:33:28</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E582" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:33:31</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D583" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E583" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:33:43</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E584" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:33:46</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E585" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:33:48</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E586" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:34:19</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E587" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:34:27</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E588" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:34:27</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E589" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:35:12</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E590" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:35:15</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E591" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:35:16</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E592" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:35:35</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>products</t>
+        </is>
+      </c>
+      <c r="D593" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E593" t="inlineStr">
+        <is>
+          <t>Opened products page</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:53:52</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E594" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:53:53</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D595" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E595" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:53:55</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D596" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E596" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:03</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E597" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:04</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D598" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E598" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:05</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E599" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:13</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E600" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:13</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E601" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:31</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E602" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:35</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E603" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:44</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E604" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:45</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E605" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:50</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E606" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:51</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E607" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:52</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E608" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:54:58</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E609" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:57:48</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E610" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:57:48</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E611" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>2025-12-24 23:57:51</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D612" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E612" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:04:56</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E613" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:04:56</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E614" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:00</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E615" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:11</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E616" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:11</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E617" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:14</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E618" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:15</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E619" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:15</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E620" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:17</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E621" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:19</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D622" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E622" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:32</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D623" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E623" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:34</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D624" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E624" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:35</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D625" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E625" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:37</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E626" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:05:40</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E627" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:07</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E628" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:08</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D629" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E629" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:09</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D630" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E630" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:20</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D631" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E631" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:28</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D632" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E632" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:34</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D633" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E633" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:38</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E634" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:42</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D635" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E635" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:13:42</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D636" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E636" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add dynamic payment terms to invoice page and template
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E636"/>
+  <dimension ref="A1:E654"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17605,6 +17605,492 @@
         </is>
       </c>
     </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:20:51</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D637" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E637" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:20:52</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E638" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:20:53</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E639" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:20:54</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E640" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:01</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E641" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:06</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>receipt</t>
+        </is>
+      </c>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E642" t="inlineStr">
+        <is>
+          <t>Opened receipt page</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:08</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E643" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:14</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E644" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:17</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E645" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:17</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E646" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:31</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E647" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:32</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E648" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:21:33</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D649" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E649" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:22:48</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E650" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:35:22</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E651" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:35:22</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E652" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:35:26</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E653" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:35:34</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E654" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove Dockerfile - using Streamlit Community Cloud
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,546 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:50:39</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:50:39</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:50:43</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:50:52</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:50:52</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:50:55</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:51:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:51:04</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:51:07</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:51:16</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:51:18</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:52:14</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:52:14</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:52:15</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:52:16</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:52:17</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:52:17</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:56:35</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:56:35</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-12-25 00:56:36</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add dynamic power provider selection for Delivery & Installation section
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,6 +1135,465 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:02:23</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:02:23</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:02:25</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:02:38</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:06:51</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:06:51</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:06:53</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:06:55</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:00</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:00</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:03</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:07</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:07</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:11</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:19</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:22</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:07:24</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add AI Product Suggester with ChatGPT integration to invoice page
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1594,6 +1594,1896 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:26</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:27</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:29</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:30</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:33</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:33</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:35</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:37</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:38</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:51</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:54</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:56</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:08:57</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:31</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:31</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:32</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:33</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:36</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:38</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:38</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:38</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:39</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:39</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:39</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:09:44</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:13</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:13</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:15</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:18</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:22</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:24</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:27</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:28</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:29</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:29</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:30</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:30</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:12:34</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:16:24</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:16:24</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:16:28</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:16:30</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:16:33</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:16:34</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:16:43</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:16:58</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:01</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:05</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:05</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:07</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:10</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:10</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:14</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:14</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:17:20</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:18:23</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:18:25</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:18:26</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:26</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:27</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:27</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:27</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:28</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:28</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:30</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:31</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:54</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:19:55</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:20:07</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:20:23</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify work details section - remove ChatGPT API, keep basic input fields only
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3484,6 +3484,195 @@
         </is>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:25:27</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:25:27</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:25:27</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:25:29</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:25:47</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:25:47</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-12-25 01:25:47</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Firebase Cloud Integration - Real-time sync for products, invoices, customers, and quotations
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-25 00:46:29</t>
+          <t>2025-12-25 02:10:21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -490,7 +490,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-25 00:46:30</t>
+          <t>2025-12-25 02:10:23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -517,7 +517,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-25 00:46:34</t>
+          <t>2025-12-25 02:10:23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-25 00:46:51</t>
+          <t>2025-12-25 02:10:41</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -571,7 +571,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-25 00:46:56</t>
+          <t>2025-12-25 02:10:44</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -598,7 +598,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-25 00:50:39</t>
+          <t>2025-12-25 02:10:44</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -608,24 +608,24 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>login_success</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Role: admin</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-25 00:50:39</t>
+          <t>2025-12-25 02:10:44</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dashboard</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -645,14 +645,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Opened dashboard page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-25 00:50:43</t>
+          <t>2025-12-25 02:10:45</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -679,7 +679,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-25 00:50:52</t>
+          <t>2025-12-25 02:10:50</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -706,7 +706,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-25 00:50:52</t>
+          <t>2025-12-25 02:10:50</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -733,7 +733,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-25 00:50:55</t>
+          <t>2025-12-25 02:10:50</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-25 00:51:00</t>
+          <t>2025-12-25 02:10:51</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -787,7 +787,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-25 00:51:04</t>
+          <t>2025-12-25 02:10:55</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -814,7 +814,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-25 00:51:07</t>
+          <t>2025-12-25 02:10:55</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -841,7 +841,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-25 00:51:16</t>
+          <t>2025-12-25 02:11:04</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-25 00:51:18</t>
+          <t>2025-12-25 02:11:24</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -895,7 +895,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-25 00:52:14</t>
+          <t>2025-12-25 02:11:30</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -922,7 +922,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-25 00:52:14</t>
+          <t>2025-12-25 02:11:31</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -949,7 +949,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-25 00:52:15</t>
+          <t>2025-12-25 02:11:32</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-25 00:52:16</t>
+          <t>2025-12-25 02:11:32</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1003,7 +1003,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-25 00:52:17</t>
+          <t>2025-12-25 02:11:34</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1030,7 +1030,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-25 00:52:17</t>
+          <t>2025-12-25 02:11:34</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1057,7 +1057,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-25 00:56:35</t>
+          <t>2025-12-25 02:11:44</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1067,24 +1067,24 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>login_success</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Role: admin</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-25 00:56:35</t>
+          <t>2025-12-25 02:11:52</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>dashboard</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1104,14 +1104,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Opened dashboard page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-25 00:56:36</t>
+          <t>2025-12-25 02:11:53</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>quotation</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1131,14 +1131,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Opened quotation page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-25 01:02:23</t>
+          <t>2025-12-25 02:11:53</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1148,24 +1148,24 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>login_success</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Role: admin</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-25 01:02:23</t>
+          <t>2025-12-25 02:12:02</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>dashboard</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1185,14 +1185,14 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Opened dashboard page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-25 01:02:25</t>
+          <t>2025-12-25 02:12:08</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>quotation</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1212,14 +1212,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Opened quotation page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-25 01:02:38</t>
+          <t>2025-12-25 02:12:08</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1246,7 +1246,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-25 01:06:51</t>
+          <t>2025-12-25 02:12:16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1256,24 +1256,24 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>login_success</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Role: admin</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-25 01:06:51</t>
+          <t>2025-12-25 02:12:23</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>dashboard</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1293,14 +1293,14 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Opened dashboard page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-25 01:06:53</t>
+          <t>2025-12-25 02:12:23</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>quotation</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1320,14 +1320,14 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Opened quotation page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-25 01:06:55</t>
+          <t>2025-12-25 02:12:27</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1354,7 +1354,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:00</t>
+          <t>2025-12-25 02:13:00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1381,7 +1381,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:00</t>
+          <t>2025-12-25 02:13:00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1408,7 +1408,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:03</t>
+          <t>2025-12-25 02:13:17</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1435,7 +1435,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:07</t>
+          <t>2025-12-25 02:13:42</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1462,7 +1462,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:07</t>
+          <t>2025-12-25 02:13:43</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1489,7 +1489,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:11</t>
+          <t>2025-12-25 02:13:56</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:19</t>
+          <t>2025-12-25 02:14:03</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1543,7 +1543,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:22</t>
+          <t>2025-12-25 02:14:03</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1570,7 +1570,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-25 01:07:24</t>
+          <t>2025-12-25 02:14:12</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1597,7 +1597,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:26</t>
+          <t>2025-12-25 02:14:13</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1607,24 +1607,24 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>login_success</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Role: admin</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:27</t>
+          <t>2025-12-25 02:14:14</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>dashboard</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1644,14 +1644,14 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Opened dashboard page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:29</t>
+          <t>2025-12-25 02:14:15</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>quotation</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1671,14 +1671,14 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Opened quotation page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:30</t>
+          <t>2025-12-25 02:14:21</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1705,7 +1705,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:33</t>
+          <t>2025-12-25 02:14:21</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1732,7 +1732,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:33</t>
+          <t>2025-12-25 02:14:27</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1759,7 +1759,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:35</t>
+          <t>2025-12-25 02:14:38</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1786,7 +1786,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:37</t>
+          <t>2025-12-25 02:14:39</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1813,7 +1813,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:38</t>
+          <t>2025-12-25 02:14:39</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:51</t>
+          <t>2025-12-25 02:14:48</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1867,7 +1867,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:54</t>
+          <t>2025-12-25 02:14:54</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1894,7 +1894,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:56</t>
+          <t>2025-12-25 02:14:56</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1921,7 +1921,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-25 01:08:57</t>
+          <t>2025-12-25 02:14:57</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1948,7 +1948,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:31</t>
+          <t>2025-12-25 02:15:07</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1975,7 +1975,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:31</t>
+          <t>2025-12-25 02:15:13</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2002,7 +2002,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:32</t>
+          <t>2025-12-25 02:15:15</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2029,7 +2029,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:33</t>
+          <t>2025-12-25 02:15:15</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2056,7 +2056,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:36</t>
+          <t>2025-12-25 02:15:31</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2083,7 +2083,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:38</t>
+          <t>2025-12-25 02:15:45</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2110,7 +2110,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:38</t>
+          <t>2025-12-25 02:15:45</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2137,7 +2137,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:38</t>
+          <t>2025-12-25 02:15:46</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2164,7 +2164,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:39</t>
+          <t>2025-12-25 02:15:53</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2191,7 +2191,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:39</t>
+          <t>2025-12-25 02:16:00</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2218,7 +2218,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:39</t>
+          <t>2025-12-25 02:16:01</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2245,7 +2245,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-25 01:09:44</t>
+          <t>2025-12-25 02:16:01</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2272,7 +2272,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:13</t>
+          <t>2025-12-25 02:16:09</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2282,24 +2282,24 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>login_success</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Role: admin</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:13</t>
+          <t>2025-12-25 02:16:15</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>dashboard</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2319,14 +2319,14 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Opened dashboard page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:15</t>
+          <t>2025-12-25 02:16:25</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2353,7 +2353,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:18</t>
+          <t>2025-12-25 02:16:29</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2380,7 +2380,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:22</t>
+          <t>2025-12-25 02:16:29</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2407,7 +2407,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:24</t>
+          <t>2025-12-25 02:16:34</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2434,7 +2434,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:27</t>
+          <t>2025-12-25 02:16:37</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2461,7 +2461,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:28</t>
+          <t>2025-12-25 02:16:37</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2488,7 +2488,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:29</t>
+          <t>2025-12-25 02:16:53</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2515,7 +2515,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:29</t>
+          <t>2025-12-25 02:16:58</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2542,7 +2542,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:30</t>
+          <t>2025-12-25 02:16:59</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2569,7 +2569,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:30</t>
+          <t>2025-12-25 02:17:13</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2596,7 +2596,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-12-25 01:12:34</t>
+          <t>2025-12-25 02:17:37</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2623,7 +2623,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-12-25 01:16:24</t>
+          <t>2025-12-25 02:17:50</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2633,24 +2633,24 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>login_success</t>
+          <t>access_granted</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Role: admin</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-12-25 01:16:24</t>
+          <t>2025-12-25 02:18:10</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>dashboard</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2670,14 +2670,14 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Opened dashboard page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-12-25 01:16:28</t>
+          <t>2025-12-25 02:18:46</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>quotation</t>
+          <t>invoice</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2697,14 +2697,14 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Opened quotation page</t>
+          <t>Opened invoice page</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-12-25 01:16:30</t>
+          <t>2025-12-25 02:21:45</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2731,7 +2731,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-12-25 01:16:33</t>
+          <t>2025-12-25 02:21:49</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2758,7 +2758,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-12-25 01:16:34</t>
+          <t>2025-12-25 02:21:54</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2785,7 +2785,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-12-25 01:16:43</t>
+          <t>2025-12-25 02:23:07</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2812,7 +2812,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-12-25 01:16:58</t>
+          <t>2025-12-25 02:23:41</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2831,843 +2831,6 @@
         </is>
       </c>
       <c r="E89" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:01</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:05</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:05</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:07</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:10</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:10</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:14</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:14</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:17:20</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:18:23</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:18:25</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:18:26</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:26</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:27</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:27</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:27</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:28</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:28</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:30</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:31</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:54</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:19:55</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>quotation</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>Opened quotation page</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:20:07</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:20:23</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:25:27</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>Login</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>login_success</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>Role: admin</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:25:27</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>dashboard</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>Opened dashboard page</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:25:27</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>dashboard</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>Opened dashboard page</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:25:29</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:25:47</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:25:47</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>Opened invoice page</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>2025-12-25 01:25:47</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>invoice</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>access_granted</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr">
         <is>
           <t>Opened invoice page</t>
         </is>

</xml_diff>

<commit_message>
Add template validation utility for placeholder extraction and validation
- Implemented functions to extract top-level placeholders from text and validate them against provided replacement keys.
- Added support for validating placeholders in HTML and DOCX files.
- Introduced error handling for missing and extra keys during validation.
- Enhanced the overall structure and readability of the template validation logic.
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2836,6 +2836,1113 @@
         </is>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:22:09</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:22:09</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:22:19</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:22:35</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:08</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:11</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:11</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:14</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:20</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:21</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:32</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:36</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:39</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:39</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:41</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:41</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:23:43</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:19</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:20</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>receipt</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Opened receipt page</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:21</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:23</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:28</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:32</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:35</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:35</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:24:37</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:25:16</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:25:18</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:25:32</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:25:36</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:28:27</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:28:45</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:27</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:27</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:30</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:34</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:35</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:36</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:42</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:47</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-12-27 13:33:53</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>invoice</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Opened invoice page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor receipt_page.py for improved readability and formatting consistency
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4753,6 +4753,168 @@
         </is>
       </c>
     </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-12-29 13:57:30</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-12-29 13:57:37</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-12-29 13:57:39</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-12-29 13:57:40</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-12-29 13:57:40</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-12-29 13:57:42</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update logs.xlsx with new data entries
</commit_message>
<xml_diff>
--- a/data/logs.xlsx
+++ b/data/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E207"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6022,6 +6022,87 @@
         </is>
       </c>
     </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2026-01-01 10:12:43</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>login_success</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>Role: admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2026-01-01 10:12:43</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>dashboard</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>Opened dashboard page</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2026-01-01 10:12:46</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>quotation</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>access_granted</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Opened quotation page</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>